<commit_message>
add cli option, update readme, split modules by responsibility
</commit_message>
<xml_diff>
--- a/input/data.xlsx
+++ b/input/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -71,6 +71,177 @@
   </si>
   <si>
     <t xml:space="preserve">Future AI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emily Brown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GHI Institute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel Wilson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LMN College</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olivia Garcia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile App Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UVW University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James Anderson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Computing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPQ Academy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sophia Martinez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer Networking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RST Institute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethan Thompson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JKL College</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chloe White</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QRS University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">William Rodriguez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blockchain Technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MNO Institute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grace Lee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UX/UI Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EFP Academy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liam Scott</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cybersecurity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WXY College</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emma Nguyen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer Vision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIJ University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aiden Perez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internet of Things</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KLM Institute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harper Turner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Privacy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PQR Academy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mia Hernandez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Big Data Analytics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XYZ College</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benjamin Flores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Embedded Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC Institute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zoe Carter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machine Learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LMN University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Henry Parker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artificial Intelligence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UVW Academy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luna Adams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python Programming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPQ College</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jackson Campbell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sofia Evans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JKL University</t>
   </si>
 </sst>
 </file>
@@ -172,13 +343,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6:E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.95"/>
@@ -256,6 +427,286 @@
       </c>
       <c r="D5" s="1" t="n">
         <v>45266</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>45058</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>45105</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>45126</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>45141</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>45194</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>45213</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>45260</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>45282</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>45308</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>45331</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>45356</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>45393</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>45420</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>45466</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>45503</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>45522</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>45549</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>45568</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>45645</v>
       </c>
     </row>
   </sheetData>

</xml_diff>